<commit_message>
Removed comments, last edits.
</commit_message>
<xml_diff>
--- a/paper_ClusterRobustTesting/CRVE_sims_table_full.xlsx
+++ b/paper_ClusterRobustTesting/CRVE_sims_table_full.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jep2963\Documents\R\clubSandwich\paper_ClusterRobustTesting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="620" windowWidth="34640" windowHeight="18600" tabRatio="500"/>
+    <workbookView xWindow="3975" yWindow="615" windowWidth="34635" windowHeight="18600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="new version" sheetId="4" r:id="rId1"/>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Simulation Review t-test'!$B$2:$R$26</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1103,6 +1108,40 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1115,30 +1154,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1154,55 +1190,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1618,98 +1623,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="5.875" customWidth="1"/>
+    <col min="3" max="3" width="6.125" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="8.375" customWidth="1"/>
+    <col min="6" max="6" width="6.625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="9" max="9" width="7.875" customWidth="1"/>
+    <col min="10" max="10" width="8.125" customWidth="1"/>
+    <col min="11" max="11" width="6.875" customWidth="1"/>
+    <col min="12" max="12" width="6.125" style="23" customWidth="1"/>
     <col min="13" max="13" width="6" style="23" customWidth="1"/>
     <col min="14" max="14" width="5.5" style="23" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" style="23" customWidth="1"/>
+    <col min="15" max="15" width="8.375" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="2:16" ht="16">
-      <c r="D4" s="58" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D4" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58" t="s">
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="59" t="s">
+      <c r="J4" s="56"/>
+      <c r="K4" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
       <c r="O4" s="39"/>
     </row>
-    <row r="5" spans="2:16" ht="15" customHeight="1">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57" t="s">
+      <c r="L5" s="69"/>
+      <c r="M5" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="N5" s="57"/>
-    </row>
-    <row r="6" spans="2:16" ht="23" customHeight="1" thickBot="1">
-      <c r="B6" s="52"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="52"/>
+      <c r="N5" s="69"/>
+    </row>
+    <row r="6" spans="2:16" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="68"/>
       <c r="K6" s="24" t="s">
         <v>60</v>
       </c>
@@ -1724,7 +1729,7 @@
       </c>
       <c r="O6"/>
     </row>
-    <row r="7" spans="2:16" ht="30">
+    <row r="7" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
         <v>62</v>
       </c>
@@ -1743,7 +1748,7 @@
       <c r="G7" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="50" t="s">
         <v>97</v>
       </c>
       <c r="I7" s="41" t="s">
@@ -1765,7 +1770,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="33" t="s">
         <v>63</v>
       </c>
@@ -1784,7 +1789,7 @@
       <c r="G8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="76" t="s">
+      <c r="H8" s="51" t="s">
         <v>98</v>
       </c>
       <c r="I8" s="13" t="s">
@@ -1806,8 +1811,8 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
-      <c r="B9" s="47" t="s">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="59" t="s">
         <v>64</v>
       </c>
       <c r="C9" s="43">
@@ -1825,7 +1830,7 @@
       <c r="G9" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="52" t="s">
         <v>99</v>
       </c>
       <c r="I9" s="43" t="s">
@@ -1851,8 +1856,8 @@
         <v>5.3000000000000047E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
-      <c r="B10" s="48"/>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="60"/>
       <c r="C10" s="45">
         <v>2</v>
       </c>
@@ -1868,7 +1873,7 @@
       <c r="G10" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="53" t="s">
         <v>99</v>
       </c>
       <c r="I10" s="45" t="s">
@@ -1894,8 +1899,8 @@
         <v>0.128</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
-      <c r="B11" s="48"/>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="60"/>
       <c r="C11" s="45">
         <v>3</v>
       </c>
@@ -1911,7 +1916,7 @@
       <c r="G11" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="78" t="s">
+      <c r="H11" s="53" t="s">
         <v>98</v>
       </c>
       <c r="I11" s="45" t="s">
@@ -1935,8 +1940,8 @@
         <v>5.3000000000000047E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
-      <c r="B12" s="48"/>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="60"/>
       <c r="C12" s="45">
         <v>4</v>
       </c>
@@ -1952,7 +1957,7 @@
       <c r="G12" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="78" t="s">
+      <c r="H12" s="53" t="s">
         <v>100</v>
       </c>
       <c r="I12" s="45" t="s">
@@ -1978,8 +1983,8 @@
         <v>5.8000000000000052E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
-      <c r="B13" s="48"/>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="60"/>
       <c r="C13" s="45">
         <v>5</v>
       </c>
@@ -1995,7 +2000,7 @@
       <c r="G13" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="78" t="s">
+      <c r="H13" s="53" t="s">
         <v>98</v>
       </c>
       <c r="I13" s="45" t="s">
@@ -2019,8 +2024,8 @@
         <v>5.3000000000000047E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
-      <c r="B14" s="48"/>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="60"/>
       <c r="C14" s="45">
         <v>5</v>
       </c>
@@ -2036,7 +2041,7 @@
       <c r="G14" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="78" t="s">
+      <c r="H14" s="53" t="s">
         <v>101</v>
       </c>
       <c r="I14" s="45" t="s">
@@ -2062,8 +2067,8 @@
         <v>5.1000000000000045E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
-      <c r="B15" s="49"/>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="61"/>
       <c r="C15" s="41">
         <v>5</v>
       </c>
@@ -2079,7 +2084,7 @@
       <c r="G15" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="75" t="s">
+      <c r="H15" s="50" t="s">
         <v>102</v>
       </c>
       <c r="I15" s="41" t="s">
@@ -2104,8 +2109,8 @@
         <v>2.9000000000000026E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
-      <c r="B16" s="47" t="s">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="59" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="43">
@@ -2123,7 +2128,7 @@
       <c r="G16" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="77" t="s">
+      <c r="H16" s="52" t="s">
         <v>98</v>
       </c>
       <c r="I16" s="43" t="s">
@@ -2132,22 +2137,22 @@
       <c r="J16" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="K16" s="70">
+      <c r="K16" s="47">
         <v>4.8099999999999997E-2</v>
       </c>
-      <c r="L16" s="70">
+      <c r="L16" s="47">
         <v>5.4899999999999997E-2</v>
       </c>
-      <c r="M16" s="70">
+      <c r="M16" s="47">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="N16" s="70">
+      <c r="N16" s="47">
         <v>5.0200000000000002E-2</v>
       </c>
       <c r="P16" s="29"/>
     </row>
-    <row r="17" spans="2:15">
-      <c r="B17" s="48"/>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="60"/>
       <c r="C17" s="45">
         <v>1</v>
       </c>
@@ -2163,7 +2168,7 @@
       <c r="G17" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="78" t="s">
+      <c r="H17" s="53" t="s">
         <v>107</v>
       </c>
       <c r="I17" s="45" t="s">
@@ -2172,21 +2177,21 @@
       <c r="J17" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="K17" s="71">
+      <c r="K17" s="48">
         <v>0.10390000000000001</v>
       </c>
-      <c r="L17" s="71">
+      <c r="L17" s="48">
         <v>0.1464</v>
       </c>
-      <c r="M17" s="72">
+      <c r="M17" s="49">
         <v>4.0599999999999997E-2</v>
       </c>
-      <c r="N17" s="72">
+      <c r="N17" s="49">
         <v>4.5400000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
-      <c r="B18" s="48"/>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="60"/>
       <c r="C18" s="45">
         <v>1</v>
       </c>
@@ -2202,7 +2207,7 @@
       <c r="G18" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="78" t="s">
+      <c r="H18" s="53" t="s">
         <v>108</v>
       </c>
       <c r="I18" s="45" t="s">
@@ -2211,21 +2216,21 @@
       <c r="J18" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="71">
+      <c r="K18" s="48">
         <v>4.8099999999999997E-2</v>
       </c>
-      <c r="L18" s="71">
+      <c r="L18" s="48">
         <v>0.19040000000000001</v>
       </c>
-      <c r="M18" s="72">
+      <c r="M18" s="49">
         <v>3.85E-2</v>
       </c>
-      <c r="N18" s="72">
+      <c r="N18" s="49">
         <v>5.79E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
-      <c r="B19" s="48"/>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="60"/>
       <c r="C19" s="45">
         <v>1</v>
       </c>
@@ -2241,7 +2246,7 @@
       <c r="G19" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="78" t="s">
+      <c r="H19" s="53" t="s">
         <v>100</v>
       </c>
       <c r="I19" s="45" t="s">
@@ -2250,21 +2255,21 @@
       <c r="J19" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="K19" s="71">
+      <c r="K19" s="48">
         <v>6.6799999999999998E-2</v>
       </c>
-      <c r="L19" s="71">
+      <c r="L19" s="48">
         <v>0.1305</v>
       </c>
-      <c r="M19" s="72">
+      <c r="M19" s="49">
         <v>3.8699999999999998E-2</v>
       </c>
-      <c r="N19" s="72">
+      <c r="N19" s="49">
         <v>4.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="48"/>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="60"/>
       <c r="C20" s="45">
         <v>1</v>
       </c>
@@ -2280,7 +2285,7 @@
       <c r="G20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="78" t="s">
+      <c r="H20" s="53" t="s">
         <v>103</v>
       </c>
       <c r="I20" s="45" t="s">
@@ -2289,21 +2294,21 @@
       <c r="J20" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="71">
+      <c r="K20" s="48">
         <v>5.6899999999999999E-2</v>
       </c>
-      <c r="L20" s="71">
+      <c r="L20" s="48">
         <v>0.1225</v>
       </c>
-      <c r="M20" s="72">
+      <c r="M20" s="49">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="N20" s="72">
+      <c r="N20" s="49">
         <v>5.5100000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:15">
-      <c r="B21" s="48"/>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="60"/>
       <c r="C21" s="45">
         <v>1</v>
       </c>
@@ -2319,7 +2324,7 @@
       <c r="G21" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="78" t="s">
+      <c r="H21" s="53" t="s">
         <v>104</v>
       </c>
       <c r="I21" s="45" t="s">
@@ -2328,21 +2333,21 @@
       <c r="J21" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="K21" s="71">
+      <c r="K21" s="48">
         <v>2.87E-2</v>
       </c>
-      <c r="L21" s="71">
+      <c r="L21" s="48">
         <v>0.28489999999999999</v>
       </c>
-      <c r="M21" s="72">
+      <c r="M21" s="49">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="N21" s="72">
+      <c r="N21" s="49">
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="30">
-      <c r="B22" s="48"/>
+    <row r="22" spans="2:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="60"/>
       <c r="C22" s="45">
         <v>2</v>
       </c>
@@ -2358,7 +2363,7 @@
       <c r="G22" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="78" t="s">
+      <c r="H22" s="53" t="s">
         <v>105</v>
       </c>
       <c r="I22" s="45" t="s">
@@ -2380,8 +2385,8 @@
         <v>6.0499999999999998E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="31" thickBot="1">
-      <c r="B23" s="50"/>
+    <row r="23" spans="2:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="62"/>
       <c r="C23" s="44">
         <v>2</v>
       </c>
@@ -2397,7 +2402,7 @@
       <c r="G23" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="79" t="s">
+      <c r="H23" s="54" t="s">
         <v>106</v>
       </c>
       <c r="I23" s="44" t="s">
@@ -2418,43 +2423,43 @@
       <c r="N23" s="30">
         <v>5.8599999999999999E-2</v>
       </c>
-      <c r="O23" s="80"/>
-    </row>
-    <row r="24" spans="2:15" ht="8" customHeight="1">
-      <c r="B24" s="53" t="s">
+      <c r="O23" s="55"/>
+    </row>
+    <row r="24" spans="2:15" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
       <c r="O24" s="38"/>
     </row>
-    <row r="25" spans="2:15" ht="83" customHeight="1">
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
+    <row r="25" spans="2:15" ht="83.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
       <c r="O25" s="38"/>
     </row>
-    <row r="26" spans="2:15" ht="45" customHeight="1">
+    <row r="26" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -2472,6 +2477,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="B24:N25"/>
     <mergeCell ref="B9:B15"/>
@@ -2488,7 +2494,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2501,7 +2506,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B3:R26"/>
@@ -2510,104 +2515,104 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.875" customWidth="1"/>
+    <col min="3" max="3" width="6.125" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="8.375" customWidth="1"/>
+    <col min="6" max="6" width="6.625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="5.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
+    <col min="10" max="10" width="6.375" customWidth="1"/>
     <col min="11" max="11" width="5.5" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" customWidth="1"/>
-    <col min="13" max="13" width="8.1640625" customWidth="1"/>
-    <col min="14" max="14" width="6.83203125" customWidth="1"/>
-    <col min="15" max="15" width="6.1640625" style="23" customWidth="1"/>
+    <col min="12" max="12" width="7.875" customWidth="1"/>
+    <col min="13" max="13" width="8.125" customWidth="1"/>
+    <col min="14" max="14" width="6.875" customWidth="1"/>
+    <col min="15" max="15" width="6.125" style="23" customWidth="1"/>
     <col min="16" max="16" width="6" style="23" customWidth="1"/>
     <col min="17" max="17" width="5.5" style="23" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" style="23" customWidth="1"/>
+    <col min="18" max="18" width="8.375" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="2:18" ht="16">
-      <c r="D4" s="58" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D4" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="60" t="s">
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="58" t="s">
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="59" t="s">
+      <c r="M4" s="56"/>
+      <c r="N4" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="70"/>
       <c r="R4" s="39"/>
     </row>
-    <row r="5" spans="2:18" ht="15" customHeight="1">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61" t="s">
+      <c r="H5" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="55" t="s">
+      <c r="K5" s="72"/>
+      <c r="L5" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="51" t="s">
+      <c r="M5" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="57" t="s">
+      <c r="N5" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57" t="s">
+      <c r="O5" s="69"/>
+      <c r="P5" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="Q5" s="57"/>
-    </row>
-    <row r="6" spans="2:18" ht="23" customHeight="1" thickBot="1">
-      <c r="B6" s="52"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="52"/>
+      <c r="Q5" s="69"/>
+    </row>
+    <row r="6" spans="2:18" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="68"/>
       <c r="H6" s="21" t="s">
         <v>79</v>
       </c>
@@ -2620,8 +2625,8 @@
       <c r="K6" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L6" s="56"/>
-      <c r="M6" s="52"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="68"/>
       <c r="N6" s="24" t="s">
         <v>60</v>
       </c>
@@ -2636,7 +2641,7 @@
       </c>
       <c r="R6"/>
     </row>
-    <row r="7" spans="2:18">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
         <v>62</v>
       </c>
@@ -2686,7 +2691,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:18">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="33" t="s">
         <v>63</v>
       </c>
@@ -2736,8 +2741,8 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:18">
-      <c r="B9" s="47" t="s">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="59" t="s">
         <v>64</v>
       </c>
       <c r="C9" s="15">
@@ -2790,8 +2795,8 @@
         <v>5.3000000000000047E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:18">
-      <c r="B10" s="48"/>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="60"/>
       <c r="C10" s="17">
         <v>2</v>
       </c>
@@ -2842,8 +2847,8 @@
         <v>0.128</v>
       </c>
     </row>
-    <row r="11" spans="2:18">
-      <c r="B11" s="48"/>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="60"/>
       <c r="C11" s="17">
         <v>3</v>
       </c>
@@ -2892,8 +2897,8 @@
         <v>5.3000000000000047E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:18">
-      <c r="B12" s="48"/>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="60"/>
       <c r="C12" s="17">
         <v>4</v>
       </c>
@@ -2944,8 +2949,8 @@
         <v>5.8000000000000052E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:18">
-      <c r="B13" s="48"/>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="60"/>
       <c r="C13" s="17">
         <v>5</v>
       </c>
@@ -2994,8 +2999,8 @@
         <v>5.3000000000000047E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:18">
-      <c r="B14" s="48"/>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="60"/>
       <c r="C14" s="17">
         <v>5</v>
       </c>
@@ -3046,8 +3051,8 @@
         <v>5.1000000000000045E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:18">
-      <c r="B15" s="49"/>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="61"/>
       <c r="C15" s="12">
         <v>5</v>
       </c>
@@ -3097,8 +3102,8 @@
         <v>2.9000000000000026E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:18">
-      <c r="B16" s="47" t="s">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="59" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="15">
@@ -3147,8 +3152,8 @@
         <v>5.4899999999999997E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:18">
-      <c r="B17" s="48"/>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="60"/>
       <c r="C17" s="17">
         <v>1</v>
       </c>
@@ -3195,8 +3200,8 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:18">
-      <c r="B18" s="48"/>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="60"/>
       <c r="C18" s="17">
         <v>1</v>
       </c>
@@ -3243,8 +3248,8 @@
         <v>6.1899999999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:18">
-      <c r="B19" s="48"/>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="60"/>
       <c r="C19" s="17">
         <v>1</v>
       </c>
@@ -3291,8 +3296,8 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:18">
-      <c r="B20" s="48"/>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="60"/>
       <c r="C20" s="17">
         <v>1</v>
       </c>
@@ -3339,8 +3344,8 @@
         <v>6.0100000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:18">
-      <c r="B21" s="48"/>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="60"/>
       <c r="C21" s="17">
         <v>1</v>
       </c>
@@ -3387,8 +3392,8 @@
         <v>0.10630000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:18">
-      <c r="B22" s="48"/>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="60"/>
       <c r="C22" s="17">
         <v>2</v>
       </c>
@@ -3435,8 +3440,8 @@
         <v>6.0499999999999998E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:18" ht="16.5" thickBot="1">
-      <c r="B23" s="50"/>
+    <row r="23" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="62"/>
       <c r="C23" s="22">
         <v>2</v>
       </c>
@@ -3483,47 +3488,47 @@
         <v>5.8599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="8" customHeight="1">
-      <c r="B24" s="53" t="s">
+    <row r="24" spans="2:18" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
-    </row>
-    <row r="25" spans="2:18" ht="83" customHeight="1">
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-    </row>
-    <row r="26" spans="2:18" ht="45" customHeight="1">
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="57"/>
+    </row>
+    <row r="25" spans="2:18" ht="83.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+    </row>
+    <row r="26" spans="2:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -3544,6 +3549,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B24:R25"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="D4:G4"/>
@@ -3555,14 +3568,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B23"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B24:R25"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3583,50 +3588,50 @@
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="13.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="11" style="5"/>
-    <col min="6" max="6" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.375" customWidth="1"/>
     <col min="7" max="9" width="11" style="2"/>
     <col min="10" max="10" width="10.5" style="2" customWidth="1"/>
     <col min="11" max="12" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
       <c r="N2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:20">
-      <c r="G3" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62" t="s">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G3" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="62"/>
-      <c r="K3" s="63" t="s">
+      <c r="J3" s="73"/>
+      <c r="K3" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63" t="s">
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="63"/>
+      <c r="O3" s="74"/>
       <c r="P3" t="s">
         <v>56</v>
       </c>
@@ -3634,7 +3639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
@@ -3734,7 +3739,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
@@ -3775,7 +3780,7 @@
         <v>0.15160000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -3816,7 +3821,7 @@
         <v>0.2344</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>1</v>
       </c>
@@ -3857,7 +3862,7 @@
         <v>0.13589999999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>1</v>
       </c>
@@ -3898,7 +3903,7 @@
         <v>9.3799999999999994E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>1</v>
       </c>
@@ -3939,7 +3944,7 @@
         <v>0.3352</v>
       </c>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>2</v>
       </c>
@@ -3986,7 +3991,7 @@
         <v>0.1249</v>
       </c>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>2</v>
       </c>
@@ -4029,7 +4034,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="31.5">
+    <row r="13" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>39</v>
       </c>
@@ -4088,7 +4093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="F14" s="1"/>
       <c r="G14" s="8"/>
@@ -4096,7 +4101,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="2:20" ht="31.5">
+    <row r="15" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
@@ -4158,7 +4163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>2</v>
       </c>
@@ -4217,7 +4222,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:20">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>3</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:20">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>4</v>
       </c>
@@ -4325,7 +4330,7 @@
         <v>6.2999999999999945E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:20">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>5</v>
       </c>
@@ -4372,7 +4377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:20">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>5</v>
       </c>
@@ -4422,7 +4427,7 @@
         <v>5.5000000000000049E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:20">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>5</v>
       </c>
@@ -4470,13 +4475,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:20">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="2:20" ht="31.5">
+    <row r="23" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>38</v>
       </c>
@@ -4561,89 +4566,89 @@
       <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="20" spans="2:19" ht="16">
-      <c r="E20" s="58" t="s">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E20" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="60" t="s">
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="69" t="s">
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="64" t="s">
+      <c r="N20" s="79"/>
+      <c r="O20" s="79"/>
+      <c r="P20" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-    </row>
-    <row r="21" spans="2:19">
-      <c r="B21" s="55" t="s">
+      <c r="Q20" s="80"/>
+      <c r="R20" s="80"/>
+      <c r="S20" s="80"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="55" t="s">
+      <c r="D21" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="55" t="s">
+      <c r="E21" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="55" t="s">
+      <c r="F21" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="55" t="s">
+      <c r="G21" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="55" t="s">
+      <c r="H21" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="I21" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61" t="s">
+      <c r="I21" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="L21" s="61"/>
-      <c r="M21" s="55" t="s">
+      <c r="L21" s="72"/>
+      <c r="M21" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="N21" s="51" t="s">
+      <c r="N21" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="O21" s="51" t="s">
+      <c r="O21" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="P21" s="57" t="s">
+      <c r="P21" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="57" t="s">
+      <c r="Q21" s="69"/>
+      <c r="R21" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="S21" s="57"/>
-    </row>
-    <row r="22" spans="2:19" ht="16.5" thickBot="1">
-      <c r="B22" s="56"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
+      <c r="S21" s="69"/>
+    </row>
+    <row r="22" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="66"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
       <c r="I22" s="21" t="s">
         <v>79</v>
       </c>
@@ -4656,9 +4661,9 @@
       <c r="L22" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="M22" s="56"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="68"/>
       <c r="P22" s="24" t="s">
         <v>60</v>
       </c>
@@ -4672,12 +4677,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="2:19" ht="16.5" thickBot="1"/>
-    <row r="24" spans="2:19">
-      <c r="B24" s="66" t="s">
+    <row r="23" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="75" t="s">
         <v>75</v>
       </c>
       <c r="D24" s="17"/>
@@ -4719,9 +4724,9 @@
       <c r="R24" s="31"/>
       <c r="S24" s="31"/>
     </row>
-    <row r="25" spans="2:19">
-      <c r="B25" s="67"/>
-      <c r="C25" s="48"/>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="77"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
         <v>71</v>
@@ -4761,9 +4766,9 @@
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
     </row>
-    <row r="26" spans="2:19">
-      <c r="B26" s="67"/>
-      <c r="C26" s="48"/>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="77"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17" t="s">
         <v>71</v>
@@ -4803,9 +4808,9 @@
       <c r="R26" s="31"/>
       <c r="S26" s="31"/>
     </row>
-    <row r="27" spans="2:19">
-      <c r="B27" s="67"/>
-      <c r="C27" s="48"/>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="77"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17" t="s">
         <v>71</v>
@@ -4845,9 +4850,9 @@
       <c r="R27" s="31"/>
       <c r="S27" s="31"/>
     </row>
-    <row r="28" spans="2:19">
-      <c r="B28" s="67"/>
-      <c r="C28" s="48"/>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="77"/>
+      <c r="C28" s="60"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17" t="s">
         <v>71</v>
@@ -4887,9 +4892,9 @@
       <c r="R28" s="31"/>
       <c r="S28" s="31"/>
     </row>
-    <row r="29" spans="2:19">
-      <c r="B29" s="67"/>
-      <c r="C29" s="48"/>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="77"/>
+      <c r="C29" s="60"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17" t="s">
         <v>71</v>
@@ -4929,9 +4934,9 @@
       <c r="R29" s="31"/>
       <c r="S29" s="31"/>
     </row>
-    <row r="30" spans="2:19" ht="16.5" thickBot="1">
-      <c r="B30" s="68"/>
-      <c r="C30" s="50"/>
+    <row r="30" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="78"/>
+      <c r="C30" s="62"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17" t="s">
         <v>71</v>
@@ -4971,11 +4976,18 @@
       <c r="R30" s="31"/>
       <c r="S30" s="31"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P20:S20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
     <mergeCell ref="C24:C30"/>
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="E20:H20"/>
@@ -4989,13 +5001,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="M21:M22"/>
-    <mergeCell ref="P20:S20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>